<commit_message>
Update DAI Municipios Enlace Transparencia.xlsx
</commit_message>
<xml_diff>
--- a/data/raw/CPLT/Request/DAI Municipios Enlace Transparencia.xlsx
+++ b/data/raw/CPLT/Request/DAI Municipios Enlace Transparencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d135da842735aabe/Escritorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3523" documentId="11_F25DC773A252ABDACC1048F3099F60CE5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75FE20B3-A399-43D7-9F99-3DA8361DEB94}"/>
+  <xr:revisionPtr revIDLastSave="3530" documentId="11_F25DC773A252ABDACC1048F3099F60CE5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7B7C285-0590-4706-8E09-4F4698AF9D4A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="804">
   <si>
     <t>Comuna</t>
   </si>
@@ -2447,6 +2447,9 @@
   </si>
   <si>
     <t>MU312T0003078</t>
+  </si>
+  <si>
+    <t>MU094T0001023</t>
   </si>
 </sst>
 </file>
@@ -2519,7 +2522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2573,6 +2576,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2858,7 +2864,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5877,8 +5883,12 @@
       <c r="B200" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="C200" s="6"/>
-      <c r="D200" s="5"/>
+      <c r="C200" s="20" t="s">
+        <v>803</v>
+      </c>
+      <c r="D200" s="13">
+        <v>44663</v>
+      </c>
       <c r="E200" s="5"/>
       <c r="F200" s="5"/>
       <c r="G200" s="5"/>

</xml_diff>